<commit_message>
fix import on mmset1
</commit_message>
<xml_diff>
--- a/test/data/mmset1-.xlsx
+++ b/test/data/mmset1-.xlsx
@@ -60,27 +60,7 @@
     <t xml:space="preserve">Generated neuron chains from sparc-nlp.ttl</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrc-model.json</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">,https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/snapshot_mmset1.json</t>
-    </r>
+    <t xml:space="preserve">https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrcm-model.json,https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/snapshot_mmset1.jsonm</t>
   </si>
   <si>
     <t xml:space="preserve">supertype</t>
@@ -1023,7 +1003,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1053,13 +1033,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -1118,11 +1091,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1132,10 +1105,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,7 +1129,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1188,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -1209,9 +1178,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrc-model"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3030,7 +2996,7 @@
       <c r="A2" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3038,7 +3004,7 @@
       <c r="A3" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3046,7 +3012,7 @@
       <c r="A4" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3054,7 +3020,7 @@
       <c r="A5" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3062,7 +3028,7 @@
       <c r="A6" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3070,7 +3036,7 @@
       <c r="A7" s="0" t="s">
         <v>307</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3078,7 +3044,7 @@
       <c r="A8" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>310</v>
       </c>
     </row>
@@ -3086,7 +3052,7 @@
       <c r="A9" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>312</v>
       </c>
     </row>
@@ -3094,7 +3060,7 @@
       <c r="A10" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>314</v>
       </c>
     </row>
@@ -3102,7 +3068,7 @@
       <c r="A11" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>316</v>
       </c>
     </row>
@@ -3110,7 +3076,7 @@
       <c r="A12" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>318</v>
       </c>
     </row>
@@ -3118,7 +3084,7 @@
       <c r="A13" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>320</v>
       </c>
     </row>
@@ -3126,7 +3092,7 @@
       <c r="A14" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>322</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix paths of mmset1 model
</commit_message>
<xml_diff>
--- a/test/data/mmset1-.xlsx
+++ b/test/data/mmset1-.xlsx
@@ -60,7 +60,7 @@
     <t xml:space="preserve">Generated neuron chains from sparc-nlp.ttl</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrcm-model.json,https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/snapshot_mmset1.jsonm</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrcm-model.json,https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/snapshot_mmset1.json</t>
   </si>
   <si>
     <t xml:space="preserve">supertype</t>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1157,7 +1157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -1178,6 +1178,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/wbrcm-model.json,https://raw.githubusercontent.com/open-physiology/open-physiology-viewer/feature/83_toggle/test/data/snapshot_mmset1.json"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>